<commit_message>
Correct name from Rex to Rex Jr.
</commit_message>
<xml_diff>
--- a/2018/com-mcas-points-20180909.xlsx
+++ b/2018/com-mcas-points-20180909.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrye/personal/autox/results/2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F1A2E73A-B196-FA4E-881E-8E8F3EF74A88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB290AF-5419-CF45-B34F-B9C8FC83922F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="460" windowWidth="18180" windowHeight="15340"/>
+    <workbookView xWindow="980" yWindow="460" windowWidth="18180" windowHeight="15340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -468,9 +468,6 @@
     <t>REX</t>
   </si>
   <si>
-    <t>SCHRULTRICH</t>
-  </si>
-  <si>
     <t>9`</t>
   </si>
   <si>
@@ -781,12 +778,15 @@
   </si>
   <si>
     <t>TERRY</t>
+  </si>
+  <si>
+    <t>SCHULTRICH JR.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="00"/>
@@ -1005,15 +1005,15 @@
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="2"/>
-    <cellStyle name="Normal 4" xfId="3"/>
-    <cellStyle name="Normal 4 2" xfId="4"/>
-    <cellStyle name="Normal 5" xfId="5"/>
-    <cellStyle name="Normal 5 2" xfId="6"/>
-    <cellStyle name="Normal 6" xfId="7"/>
-    <cellStyle name="Normal 6 2" xfId="8"/>
-    <cellStyle name="Normal 7" xfId="9"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 4 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 5" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 5 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 6" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 6 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 7" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1375,11 +1375,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IU286"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1407,10 +1407,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>242</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>243</v>
       </c>
       <c r="E1" s="10"/>
       <c r="F1" s="1"/>
@@ -1422,7 +1422,7 @@
         <v>0</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L1" s="17" t="s">
         <v>6</v>
@@ -1431,7 +1431,7 @@
         <v>4</v>
       </c>
       <c r="N1" s="25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="6.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1606,7 +1606,7 @@
         <v>27</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>121</v>
@@ -1773,7 +1773,7 @@
         <v>38</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>127</v>
@@ -2432,7 +2432,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I34" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.15">
@@ -2444,13 +2444,13 @@
       </c>
       <c r="C35" s="22"/>
       <c r="D35" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>61</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G35" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2463,7 +2463,7 @@
         <v>22</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K35" s="16">
         <v>61.332000000000001</v>
@@ -2488,13 +2488,13 @@
       </c>
       <c r="C36" s="22"/>
       <c r="D36" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E36" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>161</v>
       </c>
       <c r="G36" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2507,7 +2507,7 @@
         <v>57</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K36" s="16">
         <v>65.162000000000006</v>
@@ -2532,13 +2532,13 @@
         <v>18</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E37" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>155</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>156</v>
       </c>
       <c r="G37" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2551,7 +2551,7 @@
         <v>22</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K37" s="13">
         <v>67.02</v>
@@ -2577,13 +2577,13 @@
       </c>
       <c r="C38" s="22"/>
       <c r="D38" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>116</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G38" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2596,7 +2596,7 @@
         <v>57</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K38" s="16">
         <v>68.936000000000007</v>
@@ -2621,13 +2621,13 @@
         <v>15</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E39" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F39" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>154</v>
       </c>
       <c r="G39" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2691,7 +2691,7 @@
         <v>519</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>80</v>
@@ -2707,7 +2707,7 @@
         <v>99</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>9</v>
@@ -2734,13 +2734,13 @@
         <v>55</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>84</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G43" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2750,10 +2750,10 @@
         <v>98</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K43" s="13">
         <v>63.173000000000002</v>
@@ -2778,7 +2778,7 @@
         <v>4</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>19</v>
@@ -2794,7 +2794,7 @@
         <v>1</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J44" s="4" t="s">
         <v>62</v>
@@ -2822,13 +2822,13 @@
         <v>427</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E45" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F45" s="5" t="s">
         <v>175</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>176</v>
       </c>
       <c r="G45" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2838,7 +2838,7 @@
         <v>7</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>62</v>
@@ -2883,13 +2883,13 @@
         <v>168</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G48" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2926,13 +2926,13 @@
         <v>68</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>98</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G49" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2945,7 +2945,7 @@
         <v>22</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K49" s="13">
         <v>63.588000000000001</v>
@@ -2970,13 +2970,13 @@
         <v>460</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E50" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F50" s="5" t="s">
         <v>179</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>180</v>
       </c>
       <c r="G50" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2989,7 +2989,7 @@
         <v>22</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K50" s="13">
         <v>64.775999999999996</v>
@@ -3014,13 +3014,13 @@
         <v>517</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>100</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G51" s="5" t="str">
         <f t="shared" si="0"/>
@@ -3033,7 +3033,7 @@
         <v>22</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K51" s="13">
         <v>69.512</v>
@@ -3082,7 +3082,7 @@
         <v>97</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>37</v>
@@ -3128,16 +3128,16 @@
         <v>81</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E55" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F55" s="5" t="s">
         <v>171</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>172</v>
       </c>
       <c r="G55" s="5" t="str">
         <f t="shared" si="0"/>
@@ -3175,16 +3175,16 @@
         <v>321</v>
       </c>
       <c r="C56" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="D56" s="5" t="s">
-        <v>248</v>
-      </c>
       <c r="E56" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G56" s="5" t="str">
         <f t="shared" si="0"/>
@@ -3197,7 +3197,7 @@
         <v>22</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K56" s="16">
         <v>62.085000000000001</v>
@@ -3222,16 +3222,16 @@
         <v>688</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>115</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G57" s="5" t="str">
         <f t="shared" si="0"/>
@@ -3269,7 +3269,7 @@
         <v>990</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>83</v>
@@ -3431,10 +3431,10 @@
         <v>119</v>
       </c>
       <c r="E63" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F63" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>151</v>
       </c>
       <c r="G63" s="5" t="str">
         <f t="shared" si="0"/>
@@ -3447,7 +3447,7 @@
         <v>23</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K63" s="13">
         <v>73.364000000000004</v>
@@ -3764,26 +3764,26 @@
       </c>
       <c r="C76" s="22"/>
       <c r="D76" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E76" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F76" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="G76" s="5" t="str">
         <f t="shared" si="2"/>
         <v>CHARLES D'CRUZA</v>
       </c>
       <c r="H76" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="I76" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="I76" s="4" t="s">
+      <c r="J76" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="J76" s="4" t="s">
-        <v>167</v>
       </c>
       <c r="K76" s="13">
         <v>60.256999999999998</v>
@@ -3902,14 +3902,14 @@
         <v>146</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>147</v>
+        <v>251</v>
       </c>
       <c r="G79" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>REX SCHRULTRICH</v>
+        <v>REX SCHULTRICH JR.</v>
       </c>
       <c r="H79" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I79" s="4" t="s">
         <v>11</v>
@@ -3984,7 +3984,7 @@
       </c>
       <c r="C81" s="22"/>
       <c r="D81" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>70</v>
@@ -4028,26 +4028,26 @@
       </c>
       <c r="C82" s="4"/>
       <c r="D82" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E82" s="4" t="s">
         <v>71</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G82" s="5" t="str">
         <f t="shared" si="2"/>
         <v>TIM SUGGS</v>
       </c>
       <c r="H82" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="I82" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="I82" s="4" t="s">
+      <c r="J82" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="J82" s="4" t="s">
-        <v>167</v>
       </c>
       <c r="K82" s="13">
         <v>64.844999999999999</v>
@@ -4120,16 +4120,16 @@
         <v>79</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>26</v>
       </c>
       <c r="E86" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="F86" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="F86" s="5" t="s">
-        <v>192</v>
       </c>
       <c r="G86" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4142,7 +4142,7 @@
         <v>29</v>
       </c>
       <c r="J86" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K86" s="16">
         <v>59.63</v>
@@ -4166,7 +4166,7 @@
         <v>49</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>83</v>
@@ -4213,16 +4213,16 @@
         <v>64</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E88" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="F88" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>195</v>
       </c>
       <c r="G88" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4260,7 +4260,7 @@
         <v>134</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>38</v>
@@ -4307,16 +4307,16 @@
         <v>34</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>38</v>
       </c>
       <c r="E90" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F90" s="5" t="s">
         <v>189</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>190</v>
       </c>
       <c r="G90" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4398,7 +4398,7 @@
         <v>53</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G94" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4408,10 +4408,10 @@
         <v>76</v>
       </c>
       <c r="I94" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="J94" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="J94" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="K94" s="13">
         <v>59.56</v>
@@ -4626,7 +4626,7 @@
         <v>109</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G109" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4639,7 +4639,7 @@
         <v>73</v>
       </c>
       <c r="J109" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K109" s="13">
         <v>63.872</v>
@@ -4656,10 +4656,10 @@
         <v>25</v>
       </c>
       <c r="E110" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F110" s="5" t="s">
         <v>213</v>
-      </c>
-      <c r="F110" s="5" t="s">
-        <v>214</v>
       </c>
       <c r="G110" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4692,7 +4692,7 @@
         <v>81</v>
       </c>
       <c r="F111" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G111" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4705,7 +4705,7 @@
         <v>18</v>
       </c>
       <c r="J111" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K111" s="13">
         <v>65.462999999999994</v>
@@ -4722,10 +4722,10 @@
         <v>25</v>
       </c>
       <c r="E112" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F112" s="5" t="s">
         <v>231</v>
-      </c>
-      <c r="F112" s="5" t="s">
-        <v>232</v>
       </c>
       <c r="G112" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4755,10 +4755,10 @@
         <v>25</v>
       </c>
       <c r="E113" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="F113" s="5" t="s">
         <v>225</v>
-      </c>
-      <c r="F113" s="5" t="s">
-        <v>226</v>
       </c>
       <c r="G113" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4768,10 +4768,10 @@
         <v>13</v>
       </c>
       <c r="I113" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="J113" s="5" t="s">
         <v>227</v>
-      </c>
-      <c r="J113" s="5" t="s">
-        <v>228</v>
       </c>
       <c r="K113" s="13">
         <v>66.734999999999999</v>
@@ -4788,10 +4788,10 @@
         <v>25</v>
       </c>
       <c r="E114" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="F114" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="F114" s="5" t="s">
-        <v>203</v>
       </c>
       <c r="G114" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4804,7 +4804,7 @@
         <v>118</v>
       </c>
       <c r="J114" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K114" s="13">
         <v>67.096000000000004</v>
@@ -4821,10 +4821,10 @@
         <v>25</v>
       </c>
       <c r="E115" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="F115" s="5" t="s">
         <v>217</v>
-      </c>
-      <c r="F115" s="5" t="s">
-        <v>218</v>
       </c>
       <c r="G115" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4837,7 +4837,7 @@
         <v>22</v>
       </c>
       <c r="J115" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K115" s="13">
         <v>67.260000000000005</v>
@@ -4858,7 +4858,7 @@
         <v>84</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G116" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4888,10 +4888,10 @@
         <v>25</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G117" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4921,10 +4921,10 @@
         <v>25</v>
       </c>
       <c r="E118" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="F118" s="5" t="s">
         <v>223</v>
-      </c>
-      <c r="F118" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="G118" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4937,7 +4937,7 @@
         <v>29</v>
       </c>
       <c r="J118" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K118" s="13">
         <v>67.739000000000004</v>
@@ -4955,10 +4955,10 @@
         <v>25</v>
       </c>
       <c r="E119" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G119" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4991,7 +4991,7 @@
         <v>53</v>
       </c>
       <c r="F120" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G120" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5001,10 +5001,10 @@
         <v>4</v>
       </c>
       <c r="I120" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="J120" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="J120" s="5" t="s">
-        <v>211</v>
       </c>
       <c r="K120" s="13">
         <v>68.902000000000001</v>
@@ -5021,10 +5021,10 @@
         <v>25</v>
       </c>
       <c r="E121" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F121" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="F121" s="5" t="s">
-        <v>198</v>
       </c>
       <c r="G121" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5057,7 +5057,7 @@
         <v>13</v>
       </c>
       <c r="F122" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G122" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5087,10 +5087,10 @@
         <v>25</v>
       </c>
       <c r="E123" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="F123" s="5" t="s">
         <v>220</v>
-      </c>
-      <c r="F123" s="5" t="s">
-        <v>221</v>
       </c>
       <c r="G123" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5103,7 +5103,7 @@
         <v>17</v>
       </c>
       <c r="J123" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K123" s="13">
         <v>69.13</v>
@@ -5120,10 +5120,10 @@
         <v>25</v>
       </c>
       <c r="E124" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="F124" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="F124" s="5" t="s">
-        <v>206</v>
       </c>
       <c r="G124" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5154,10 +5154,10 @@
         <v>25</v>
       </c>
       <c r="E125" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F125" s="5" t="s">
         <v>235</v>
-      </c>
-      <c r="F125" s="5" t="s">
-        <v>236</v>
       </c>
       <c r="G125" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5170,7 +5170,7 @@
         <v>12</v>
       </c>
       <c r="J125" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K125" s="13">
         <v>71.132999999999996</v>
@@ -5190,7 +5190,7 @@
         <v>122</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G126" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5223,7 +5223,7 @@
         <v>80</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G127" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5236,7 +5236,7 @@
         <v>22</v>
       </c>
       <c r="J127" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K127" s="13">
         <v>75.64</v>
@@ -5254,10 +5254,10 @@
         <v>25</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G128" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5288,10 +5288,10 @@
         <v>25</v>
       </c>
       <c r="E129" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G129" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8784,7 +8784,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -8801,7 +8801,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Fix misspelling of Stu's name.
</commit_message>
<xml_diff>
--- a/2018/com-mcas-points-20180909.xlsx
+++ b/2018/com-mcas-points-20180909.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrye/personal/autox/results/2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DC6A5B-1FA8-144E-A9CB-7343C0A3B6FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC15C51E-766A-334B-8EC1-52C28CE3327A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="460" windowWidth="18180" windowHeight="15340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="253">
   <si>
     <t>CAR</t>
   </si>
@@ -168,9 +168,6 @@
     <t>MR2</t>
   </si>
   <si>
-    <t>NABOR</t>
-  </si>
-  <si>
     <t>RON</t>
   </si>
   <si>
@@ -781,6 +778,12 @@
   </si>
   <si>
     <t>D'CRUZ</t>
+  </si>
+  <si>
+    <t>STUART</t>
+  </si>
+  <si>
+    <t>NABER</t>
   </si>
 </sst>
 </file>
@@ -1378,8 +1381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IU286"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1407,10 +1410,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>240</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>241</v>
       </c>
       <c r="E1" s="10"/>
       <c r="F1" s="1"/>
@@ -1422,7 +1425,7 @@
         <v>0</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L1" s="17" t="s">
         <v>6</v>
@@ -1431,7 +1434,7 @@
         <v>4</v>
       </c>
       <c r="N1" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="6.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1455,7 +1458,7 @@
       <c r="G3" s="5"/>
       <c r="H3" s="19"/>
       <c r="I3" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="16"/>
@@ -1475,7 +1478,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G4" s="5" t="str">
         <f>E4&amp;" "&amp;F4</f>
@@ -1488,7 +1491,7 @@
         <v>23</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K4" s="13">
         <v>63.179000000000002</v>
@@ -1532,7 +1535,7 @@
         <v>23</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K5" s="16">
         <v>65.260000000000005</v>
@@ -1561,10 +1564,10 @@
         <v>27</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G6" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1577,7 +1580,7 @@
         <v>23</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K6" s="16">
         <v>66.525000000000006</v>
@@ -1606,10 +1609,10 @@
         <v>27</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G7" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1622,7 +1625,7 @@
         <v>23</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K7" s="16">
         <v>68.736000000000004</v>
@@ -1668,7 +1671,7 @@
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="16"/>
@@ -1685,10 +1688,10 @@
         <v>38</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G10" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1701,7 +1704,7 @@
         <v>16</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K10" s="16">
         <v>61.847000000000001</v>
@@ -1773,10 +1776,10 @@
         <v>38</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G12" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1789,7 +1792,7 @@
         <v>16</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K12" s="16">
         <v>63.354999999999997</v>
@@ -1818,10 +1821,10 @@
         <v>38</v>
       </c>
       <c r="E13" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>123</v>
       </c>
       <c r="G13" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1834,7 +1837,7 @@
         <v>18</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K13" s="16">
         <v>63.545999999999999</v>
@@ -1863,10 +1866,10 @@
         <v>38</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G14" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1876,10 +1879,10 @@
         <v>1</v>
       </c>
       <c r="I14" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="K14" s="16">
         <v>65.013000000000005</v>
@@ -1910,7 +1913,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I16" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.15">
@@ -1937,7 +1940,7 @@
         <v>13</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>15</v>
@@ -1968,10 +1971,10 @@
         <v>28</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G18" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1981,10 +1984,10 @@
         <v>15</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K18" s="16">
         <v>65.031000000000006</v>
@@ -2013,10 +2016,10 @@
         <v>28</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G19" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2029,7 +2032,7 @@
         <v>18</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K19" s="16">
         <v>67.453999999999994</v>
@@ -2060,7 +2063,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I21" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.15">
@@ -2072,13 +2075,13 @@
       </c>
       <c r="C22" s="22"/>
       <c r="D22" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E22" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="G22" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2091,7 +2094,7 @@
         <v>16</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K22" s="16">
         <v>65.37</v>
@@ -2115,13 +2118,13 @@
         <v>117</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G23" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2131,10 +2134,10 @@
         <v>5</v>
       </c>
       <c r="I23" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="J23" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>140</v>
       </c>
       <c r="K23" s="13">
         <v>65.772999999999996</v>
@@ -2159,13 +2162,13 @@
         <v>154</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G24" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2175,10 +2178,10 @@
         <v>13</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K24" s="13">
         <v>66.572999999999993</v>
@@ -2209,7 +2212,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I26" s="26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.15">
@@ -2224,10 +2227,10 @@
         <v>45</v>
       </c>
       <c r="E27" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="G27" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2268,10 +2271,10 @@
         <v>45</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G28" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2313,14 +2316,14 @@
         <v>45</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>26</v>
+        <v>251</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>47</v>
+        <v>252</v>
       </c>
       <c r="G29" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>STU NABOR</v>
+        <v>STUART NABER</v>
       </c>
       <c r="H29" s="19">
         <v>5</v>
@@ -2355,10 +2358,10 @@
         <v>45</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G30" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2432,7 +2435,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I34" s="26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.15">
@@ -2444,13 +2447,13 @@
       </c>
       <c r="C35" s="22"/>
       <c r="D35" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G35" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2463,7 +2466,7 @@
         <v>22</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K35" s="16">
         <v>61.332000000000001</v>
@@ -2488,13 +2491,13 @@
       </c>
       <c r="C36" s="22"/>
       <c r="D36" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E36" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>160</v>
       </c>
       <c r="G36" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2504,10 +2507,10 @@
         <v>5</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K36" s="16">
         <v>65.162000000000006</v>
@@ -2532,13 +2535,13 @@
         <v>18</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E37" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>154</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>155</v>
       </c>
       <c r="G37" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2551,7 +2554,7 @@
         <v>22</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K37" s="13">
         <v>67.02</v>
@@ -2577,13 +2580,13 @@
       </c>
       <c r="C38" s="22"/>
       <c r="D38" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G38" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2593,10 +2596,10 @@
         <v>5</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K38" s="16">
         <v>68.936000000000007</v>
@@ -2621,13 +2624,13 @@
         <v>15</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E39" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F39" s="5" t="s">
         <v>152</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>153</v>
       </c>
       <c r="G39" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2640,7 +2643,7 @@
         <v>22</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K39" s="13">
         <v>70.400000000000006</v>
@@ -2679,7 +2682,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I41" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J41" s="4"/>
     </row>
@@ -2691,13 +2694,13 @@
         <v>519</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G42" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2707,7 +2710,7 @@
         <v>99</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>9</v>
@@ -2734,13 +2737,13 @@
         <v>55</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G43" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2750,10 +2753,10 @@
         <v>98</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K43" s="13">
         <v>63.173000000000002</v>
@@ -2778,7 +2781,7 @@
         <v>4</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>19</v>
@@ -2794,10 +2797,10 @@
         <v>1</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K44" s="13">
         <v>67.679000000000002</v>
@@ -2822,13 +2825,13 @@
         <v>427</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E45" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F45" s="5" t="s">
         <v>173</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>174</v>
       </c>
       <c r="G45" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2838,10 +2841,10 @@
         <v>7</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K45" s="13">
         <v>73.114999999999995</v>
@@ -2872,7 +2875,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I47" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.15">
@@ -2883,13 +2886,13 @@
         <v>168</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G48" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2902,7 +2905,7 @@
         <v>23</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K48" s="13">
         <v>62.470999999999997</v>
@@ -2926,13 +2929,13 @@
         <v>68</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G49" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2945,7 +2948,7 @@
         <v>22</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K49" s="13">
         <v>63.588000000000001</v>
@@ -2970,13 +2973,13 @@
         <v>460</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E50" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F50" s="5" t="s">
         <v>177</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>178</v>
       </c>
       <c r="G50" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2989,7 +2992,7 @@
         <v>22</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K50" s="13">
         <v>64.775999999999996</v>
@@ -3014,13 +3017,13 @@
         <v>517</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G51" s="5" t="str">
         <f t="shared" si="0"/>
@@ -3033,7 +3036,7 @@
         <v>22</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K51" s="13">
         <v>69.512</v>
@@ -3069,7 +3072,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I53" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J53" s="20"/>
       <c r="K53" s="20"/>
@@ -3082,16 +3085,16 @@
         <v>97</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>37</v>
       </c>
       <c r="E54" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F54" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="G54" s="5" t="str">
         <f t="shared" si="0"/>
@@ -3104,7 +3107,7 @@
         <v>22</v>
       </c>
       <c r="J54" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K54" s="13">
         <v>63.241</v>
@@ -3128,16 +3131,16 @@
         <v>81</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E55" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F55" s="5" t="s">
         <v>169</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>170</v>
       </c>
       <c r="G55" s="5" t="str">
         <f t="shared" si="0"/>
@@ -3175,16 +3178,16 @@
         <v>321</v>
       </c>
       <c r="C56" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="D56" s="5" t="s">
-        <v>246</v>
-      </c>
       <c r="E56" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G56" s="5" t="str">
         <f t="shared" si="0"/>
@@ -3197,7 +3200,7 @@
         <v>22</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K56" s="16">
         <v>62.085000000000001</v>
@@ -3222,16 +3225,16 @@
         <v>688</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G57" s="5" t="str">
         <f t="shared" si="0"/>
@@ -3241,10 +3244,10 @@
         <v>15</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K57" s="13">
         <v>62.566000000000003</v>
@@ -3269,16 +3272,16 @@
         <v>990</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G58" s="5" t="str">
         <f t="shared" si="0"/>
@@ -3384,13 +3387,13 @@
       </c>
       <c r="C62" s="22"/>
       <c r="D62" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E62" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F62" s="5" t="s">
         <v>142</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>143</v>
       </c>
       <c r="G62" s="5" t="str">
         <f t="shared" si="0"/>
@@ -3403,7 +3406,7 @@
         <v>23</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K62" s="13">
         <v>69.293999999999997</v>
@@ -3428,13 +3431,13 @@
       </c>
       <c r="C63" s="22"/>
       <c r="D63" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E63" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F63" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="G63" s="5" t="str">
         <f t="shared" si="0"/>
@@ -3447,7 +3450,7 @@
         <v>23</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K63" s="13">
         <v>73.364000000000004</v>
@@ -3587,13 +3590,13 @@
         <v>19</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G72" s="5" t="str">
         <f t="shared" si="2"/>
@@ -3634,10 +3637,10 @@
         <v>26</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G73" s="5" t="str">
         <f t="shared" si="2"/>
@@ -3650,7 +3653,7 @@
         <v>18</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K73" s="13">
         <v>63.9</v>
@@ -3678,10 +3681,10 @@
         <v>3</v>
       </c>
       <c r="E74" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F74" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="G74" s="5" t="str">
         <f t="shared" si="2"/>
@@ -3719,13 +3722,13 @@
       </c>
       <c r="C75" s="22"/>
       <c r="D75" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E75" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F75" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>145</v>
       </c>
       <c r="G75" s="5" t="str">
         <f t="shared" si="2"/>
@@ -3764,26 +3767,26 @@
       </c>
       <c r="C76" s="22"/>
       <c r="D76" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G76" s="5" t="str">
         <f t="shared" si="2"/>
         <v>CHARLES D'CRUZ</v>
       </c>
       <c r="H76" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="I76" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="I76" s="4" t="s">
+      <c r="J76" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="J76" s="4" t="s">
-        <v>166</v>
       </c>
       <c r="K76" s="13">
         <v>60.256999999999998</v>
@@ -3808,13 +3811,13 @@
       </c>
       <c r="C77" s="22"/>
       <c r="D77" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E77" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F77" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="G77" s="5" t="str">
         <f t="shared" si="2"/>
@@ -3827,7 +3830,7 @@
         <v>29</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K77" s="13">
         <v>65.367000000000004</v>
@@ -3852,13 +3855,13 @@
       </c>
       <c r="C78" s="22"/>
       <c r="D78" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E78" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F78" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>75</v>
       </c>
       <c r="G78" s="5" t="str">
         <f t="shared" si="2"/>
@@ -3868,10 +3871,10 @@
         <v>5</v>
       </c>
       <c r="I78" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J78" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="J78" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="K78" s="13">
         <v>63.356000000000002</v>
@@ -3896,20 +3899,20 @@
       </c>
       <c r="C79" s="22"/>
       <c r="D79" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G79" s="5" t="str">
         <f t="shared" si="2"/>
         <v>REX SCHULTRICH JR.</v>
       </c>
       <c r="H79" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I79" s="4" t="s">
         <v>11</v>
@@ -3940,13 +3943,13 @@
         <v>27</v>
       </c>
       <c r="D80" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E80" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E80" s="4" t="s">
+      <c r="F80" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="G80" s="5" t="str">
         <f t="shared" si="2"/>
@@ -3959,7 +3962,7 @@
         <v>12</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K80" s="13">
         <v>66.337999999999994</v>
@@ -3984,13 +3987,13 @@
       </c>
       <c r="C81" s="22"/>
       <c r="D81" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G81" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4028,26 +4031,26 @@
       </c>
       <c r="C82" s="4"/>
       <c r="D82" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F82" s="5" t="s">
         <v>162</v>
-      </c>
-      <c r="E82" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>163</v>
       </c>
       <c r="G82" s="5" t="str">
         <f t="shared" si="2"/>
         <v>TIM SUGGS</v>
       </c>
       <c r="H82" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="I82" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="I82" s="4" t="s">
+      <c r="J82" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="J82" s="4" t="s">
-        <v>166</v>
       </c>
       <c r="K82" s="13">
         <v>64.844999999999999</v>
@@ -4120,16 +4123,16 @@
         <v>79</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>26</v>
       </c>
       <c r="E86" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="F86" s="5" t="s">
         <v>189</v>
-      </c>
-      <c r="F86" s="5" t="s">
-        <v>190</v>
       </c>
       <c r="G86" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4142,7 +4145,7 @@
         <v>29</v>
       </c>
       <c r="J86" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K86" s="16">
         <v>59.63</v>
@@ -4166,16 +4169,16 @@
         <v>49</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E87" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F87" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="G87" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4188,7 +4191,7 @@
         <v>11</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K87" s="13">
         <v>59.743000000000002</v>
@@ -4213,16 +4216,16 @@
         <v>64</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E88" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F88" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>193</v>
       </c>
       <c r="G88" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4260,7 +4263,7 @@
         <v>134</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>38</v>
@@ -4269,7 +4272,7 @@
         <v>24</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G89" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4282,7 +4285,7 @@
         <v>17</v>
       </c>
       <c r="J89" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K89" s="13">
         <v>62.024999999999999</v>
@@ -4307,16 +4310,16 @@
         <v>34</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>38</v>
       </c>
       <c r="E90" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F90" s="5" t="s">
         <v>187</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>188</v>
       </c>
       <c r="G90" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4329,7 +4332,7 @@
         <v>17</v>
       </c>
       <c r="J90" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K90" s="13">
         <v>69.611999999999995</v>
@@ -4379,7 +4382,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I93" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J93" s="5"/>
     </row>
@@ -4392,13 +4395,13 @@
       </c>
       <c r="C94" s="4"/>
       <c r="D94" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E94" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E94" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="F94" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G94" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4408,10 +4411,10 @@
         <v>76</v>
       </c>
       <c r="I94" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="J94" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="J94" s="4" t="s">
-        <v>186</v>
       </c>
       <c r="K94" s="13">
         <v>59.56</v>
@@ -4623,10 +4626,10 @@
         <v>25</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G109" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4636,10 +4639,10 @@
         <v>4</v>
       </c>
       <c r="I109" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J109" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K109" s="13">
         <v>63.872</v>
@@ -4656,10 +4659,10 @@
         <v>25</v>
       </c>
       <c r="E110" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="F110" s="5" t="s">
         <v>211</v>
-      </c>
-      <c r="F110" s="5" t="s">
-        <v>212</v>
       </c>
       <c r="G110" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4689,10 +4692,10 @@
         <v>25</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F111" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G111" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4705,7 +4708,7 @@
         <v>18</v>
       </c>
       <c r="J111" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K111" s="13">
         <v>65.462999999999994</v>
@@ -4722,10 +4725,10 @@
         <v>25</v>
       </c>
       <c r="E112" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="F112" s="5" t="s">
         <v>229</v>
-      </c>
-      <c r="F112" s="5" t="s">
-        <v>230</v>
       </c>
       <c r="G112" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4755,10 +4758,10 @@
         <v>25</v>
       </c>
       <c r="E113" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="F113" s="5" t="s">
         <v>223</v>
-      </c>
-      <c r="F113" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="G113" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4768,10 +4771,10 @@
         <v>13</v>
       </c>
       <c r="I113" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="J113" s="5" t="s">
         <v>225</v>
-      </c>
-      <c r="J113" s="5" t="s">
-        <v>226</v>
       </c>
       <c r="K113" s="13">
         <v>66.734999999999999</v>
@@ -4788,10 +4791,10 @@
         <v>25</v>
       </c>
       <c r="E114" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="F114" s="5" t="s">
         <v>200</v>
-      </c>
-      <c r="F114" s="5" t="s">
-        <v>201</v>
       </c>
       <c r="G114" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4801,10 +4804,10 @@
         <v>99</v>
       </c>
       <c r="I114" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J114" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K114" s="13">
         <v>67.096000000000004</v>
@@ -4821,10 +4824,10 @@
         <v>25</v>
       </c>
       <c r="E115" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F115" s="5" t="s">
         <v>215</v>
-      </c>
-      <c r="F115" s="5" t="s">
-        <v>216</v>
       </c>
       <c r="G115" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4837,7 +4840,7 @@
         <v>22</v>
       </c>
       <c r="J115" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K115" s="13">
         <v>67.260000000000005</v>
@@ -4855,10 +4858,10 @@
         <v>25</v>
       </c>
       <c r="E116" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G116" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4871,7 +4874,7 @@
         <v>22</v>
       </c>
       <c r="J116" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K116" s="13">
         <v>67.552999999999997</v>
@@ -4888,10 +4891,10 @@
         <v>25</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G117" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4904,7 +4907,7 @@
         <v>22</v>
       </c>
       <c r="J117" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K117" s="13">
         <v>67.602999999999994</v>
@@ -4921,10 +4924,10 @@
         <v>25</v>
       </c>
       <c r="E118" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="F118" s="5" t="s">
         <v>221</v>
-      </c>
-      <c r="F118" s="5" t="s">
-        <v>222</v>
       </c>
       <c r="G118" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4937,7 +4940,7 @@
         <v>29</v>
       </c>
       <c r="J118" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K118" s="13">
         <v>67.739000000000004</v>
@@ -4955,10 +4958,10 @@
         <v>25</v>
       </c>
       <c r="E119" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G119" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4988,10 +4991,10 @@
         <v>25</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F120" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G120" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5001,10 +5004,10 @@
         <v>4</v>
       </c>
       <c r="I120" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="J120" s="5" t="s">
         <v>208</v>
-      </c>
-      <c r="J120" s="5" t="s">
-        <v>209</v>
       </c>
       <c r="K120" s="13">
         <v>68.902000000000001</v>
@@ -5021,10 +5024,10 @@
         <v>25</v>
       </c>
       <c r="E121" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="F121" s="5" t="s">
         <v>195</v>
-      </c>
-      <c r="F121" s="5" t="s">
-        <v>196</v>
       </c>
       <c r="G121" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5037,7 +5040,7 @@
         <v>22</v>
       </c>
       <c r="J121" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K121" s="13">
         <v>69.004000000000005</v>
@@ -5057,7 +5060,7 @@
         <v>13</v>
       </c>
       <c r="F122" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G122" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5070,7 +5073,7 @@
         <v>23</v>
       </c>
       <c r="J122" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K122" s="13">
         <v>69.06</v>
@@ -5087,10 +5090,10 @@
         <v>25</v>
       </c>
       <c r="E123" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F123" s="5" t="s">
         <v>218</v>
-      </c>
-      <c r="F123" s="5" t="s">
-        <v>219</v>
       </c>
       <c r="G123" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5103,7 +5106,7 @@
         <v>17</v>
       </c>
       <c r="J123" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K123" s="13">
         <v>69.13</v>
@@ -5120,10 +5123,10 @@
         <v>25</v>
       </c>
       <c r="E124" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F124" s="5" t="s">
         <v>203</v>
-      </c>
-      <c r="F124" s="5" t="s">
-        <v>204</v>
       </c>
       <c r="G124" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5136,7 +5139,7 @@
         <v>18</v>
       </c>
       <c r="J124" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K124" s="13">
         <v>69.257999999999996</v>
@@ -5154,10 +5157,10 @@
         <v>25</v>
       </c>
       <c r="E125" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="F125" s="5" t="s">
         <v>233</v>
-      </c>
-      <c r="F125" s="5" t="s">
-        <v>234</v>
       </c>
       <c r="G125" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5170,7 +5173,7 @@
         <v>12</v>
       </c>
       <c r="J125" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K125" s="13">
         <v>71.132999999999996</v>
@@ -5187,10 +5190,10 @@
         <v>25</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G126" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5203,7 +5206,7 @@
         <v>23</v>
       </c>
       <c r="J126" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K126" s="13">
         <v>73.003</v>
@@ -5220,10 +5223,10 @@
         <v>25</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G127" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5236,7 +5239,7 @@
         <v>22</v>
       </c>
       <c r="J127" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K127" s="13">
         <v>75.64</v>
@@ -5254,10 +5257,10 @@
         <v>25</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G128" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5288,10 +5291,10 @@
         <v>25</v>
       </c>
       <c r="E129" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G129" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5304,7 +5307,7 @@
         <v>22</v>
       </c>
       <c r="J129" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K129" s="13">
         <v>82.727000000000004</v>
@@ -8772,7 +8775,7 @@
     </row>
     <row r="286" spans="1:14" x14ac:dyDescent="0.15">
       <c r="I286" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>